<commit_message>
File Modifications for excel and TestBase.
</commit_message>
<xml_diff>
--- a/PearlWebAutomation/src/test/resources/TestData.xlsx
+++ b/PearlWebAutomation/src/test/resources/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19020" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19020" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -120,6 +120,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -167,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,7 +205,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
@@ -505,9 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Committing... New Framework changes...
</commit_message>
<xml_diff>
--- a/PearlWebAutomation/src/test/resources/TestData.xlsx
+++ b/PearlWebAutomation/src/test/resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>formSubmitionVerification</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muzzafar </t>
+  </si>
+  <si>
+    <t>Sufyan</t>
+  </si>
+  <si>
+    <t>formSubmitionVerification-US AMRKET</t>
   </si>
 </sst>
 </file>
@@ -84,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,10 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,25 +430,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -481,24 +498,87 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>